<commit_message>
Used for teting lenses. Works.
</commit_message>
<xml_diff>
--- a/Docs/Camera module overview.xlsx
+++ b/Docs/Camera module overview.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Camera sensor" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="Calculation" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Lenses!$A$5:$K$26</definedName>
     <definedName name="aspect">Calculation!$B$8</definedName>
     <definedName name="ccd_h">Calculation!$B$7</definedName>
     <definedName name="ccd_w">Calculation!$B$6</definedName>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
   <si>
     <t>Technical specs comparison</t>
   </si>
@@ -508,6 +509,24 @@
   </si>
   <si>
     <t>1.8/6mm (default linse)</t>
+  </si>
+  <si>
+    <t>Lense #</t>
+  </si>
+  <si>
+    <t>afstand cm</t>
+  </si>
+  <si>
+    <t>left cm</t>
+  </si>
+  <si>
+    <t>right cm</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>view width</t>
   </si>
 </sst>
 </file>
@@ -667,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -738,6 +757,16 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1677,10 +1706,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:K26"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1693,7 +1722,7 @@
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="28.5">
+    <row r="1" spans="1:17">
       <c r="A1" s="29" t="s">
         <v>63</v>
       </c>
@@ -1712,7 +1741,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1">
       <c r="A2" s="30"/>
       <c r="B2" s="16" t="s">
         <v>64</v>
@@ -1727,7 +1756,7 @@
       <c r="F2" s="31"/>
       <c r="G2" s="30"/>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:17">
       <c r="A3" s="30"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
@@ -1742,7 +1771,7 @@
       </c>
       <c r="G3" s="30"/>
     </row>
-    <row r="4" spans="1:11" ht="43.5" thickBot="1">
+    <row r="4" spans="1:17" ht="43.5" thickBot="1">
       <c r="A4" s="31"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
@@ -1762,66 +1791,84 @@
       <c r="K4" s="27" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1">
+      <c r="L4" t="s">
+        <v>122</v>
+      </c>
+      <c r="M4" t="s">
+        <v>123</v>
+      </c>
+      <c r="N4" t="s">
+        <v>124</v>
+      </c>
+      <c r="O4" t="s">
+        <v>125</v>
+      </c>
+      <c r="P4" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" thickBot="1">
       <c r="A5" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="32">
         <v>3.2</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="32">
         <v>68</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="32">
         <v>51</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="32">
         <v>85</v>
       </c>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1">
+    <row r="6" spans="1:17" ht="15.75" thickBot="1">
       <c r="A6" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="32">
         <v>2.8</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="32">
         <v>90</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="32">
         <v>68</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="32">
         <v>112</v>
       </c>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1">
+    <row r="7" spans="1:17" ht="15.75" thickBot="1">
       <c r="A7" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="32">
         <v>2.6</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="32">
         <v>90</v>
       </c>
-      <c r="E7" s="17">
+      <c r="E7" s="32">
         <v>68</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="32">
         <v>112</v>
       </c>
       <c r="G7" s="17"/>
@@ -1833,416 +1880,806 @@
         <v>3.5135135135135136</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
+    <row r="8" spans="1:17" ht="15.75" thickBot="1">
       <c r="A8" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="32">
         <v>2.8</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="32">
         <v>90</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="32">
         <v>68</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="32">
         <v>112</v>
       </c>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+    <row r="9" spans="1:17" ht="15.75" thickBot="1">
       <c r="A9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="32">
         <v>1.8</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="32">
         <v>104</v>
       </c>
-      <c r="E9" s="17">
+      <c r="E9" s="32">
         <v>78</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="32">
         <v>130</v>
       </c>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1">
+    <row r="10" spans="1:17" ht="15.75" thickBot="1">
       <c r="A10" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="32">
         <v>6</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="32">
         <v>48</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="32">
         <v>36</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="32">
         <v>60</v>
       </c>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1">
+    <row r="11" spans="1:17" ht="15.75" thickBot="1">
       <c r="A11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="32">
         <v>8</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="32">
         <v>36</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="32">
         <v>27</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="32">
         <v>45</v>
       </c>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1">
+    <row r="12" spans="1:17" ht="15.75" thickBot="1">
       <c r="A12" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="32">
         <v>12</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="32">
         <v>20</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="32">
         <v>15</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="32">
         <v>25</v>
       </c>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1">
+    <row r="13" spans="1:17" ht="15.75" thickBot="1">
       <c r="A13" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="32">
         <v>10</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="32">
         <v>18</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="32">
         <v>13</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="32">
         <v>22</v>
       </c>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+    <row r="14" spans="1:17" ht="15.75" thickBot="1">
       <c r="A14" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="32">
         <v>2.8</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="32">
         <v>96</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="32">
         <v>72</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="32">
         <v>120</v>
       </c>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+    <row r="15" spans="1:17" ht="15.75" thickBot="1">
       <c r="A15" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="17" t="s">
+      <c r="B15" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="32">
         <v>2.1</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="32">
         <v>116</v>
       </c>
-      <c r="E15" s="17">
+      <c r="E15" s="32">
         <v>87</v>
       </c>
-      <c r="F15" s="17">
+      <c r="F15" s="32">
         <v>145</v>
       </c>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:17" ht="15.75" thickBot="1">
       <c r="A16" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="32">
         <v>2.25</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="32">
         <v>136</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="32">
         <v>102</v>
       </c>
-      <c r="F16" s="17">
+      <c r="F16" s="32">
         <v>170</v>
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:7" ht="15.75" thickBot="1">
+    <row r="17" spans="1:17" ht="15.75" thickBot="1">
       <c r="A17" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="32" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="32">
         <v>4</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="32">
         <v>84</v>
       </c>
-      <c r="E17" s="17">
+      <c r="E17" s="32">
         <v>63</v>
       </c>
-      <c r="F17" s="17">
+      <c r="F17" s="32">
         <v>105</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:7" ht="15.75" thickBot="1">
+    <row r="18" spans="1:17" ht="15.75" thickBot="1">
       <c r="A18" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="32">
         <v>3.8</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="32">
         <v>85</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="32">
         <v>64</v>
       </c>
-      <c r="F18" s="17">
+      <c r="F18" s="32">
         <v>106</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1">
+    <row r="19" spans="1:17" ht="15.75" thickBot="1">
       <c r="A19" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="32">
         <v>2.8</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="32">
         <v>110</v>
       </c>
-      <c r="E19" s="17">
+      <c r="E19" s="32">
         <v>83</v>
       </c>
-      <c r="F19" s="17">
+      <c r="F19" s="32">
         <v>138</v>
       </c>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1">
+    <row r="20" spans="1:17" ht="15.75" thickBot="1">
       <c r="A20" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="32">
         <v>3</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="32">
         <v>112</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="32">
         <v>84</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="32">
         <v>140</v>
       </c>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1">
+    <row r="21" spans="1:17" ht="15.75" thickBot="1">
       <c r="A21" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="32">
         <v>2.8</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="32">
         <v>124</v>
       </c>
-      <c r="E21" s="17">
+      <c r="E21" s="32">
         <v>93</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="32">
         <v>155</v>
       </c>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:7" ht="15.75" thickBot="1">
+    <row r="22" spans="1:17" ht="15.75" thickBot="1">
       <c r="A22" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="32">
         <v>1.56</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="32">
         <v>191</v>
       </c>
-      <c r="E22" s="17">
+      <c r="E22" s="32">
         <v>127</v>
       </c>
-      <c r="F22" s="17">
+      <c r="F22" s="32">
         <v>204</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="15.75" thickBot="1">
+    <row r="23" spans="1:17" ht="15.75" thickBot="1">
       <c r="A23" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="17">
+      <c r="C23" s="32">
         <v>1.05</v>
       </c>
-      <c r="D23" s="17">
+      <c r="D23" s="32">
         <v>194</v>
       </c>
-      <c r="E23" s="17">
+      <c r="E23" s="32">
         <v>142</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="32">
         <v>206</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1">
+    <row r="24" spans="1:17" ht="15.75" thickBot="1">
       <c r="A24" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="17">
+      <c r="C24" s="32">
         <v>1.58</v>
       </c>
-      <c r="D24" s="17">
+      <c r="D24" s="32">
         <v>185</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="32">
         <v>139</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="32">
         <v>200</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15.75" thickBot="1">
+    <row r="25" spans="1:17" ht="15.75" thickBot="1">
       <c r="A25" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="17" t="s">
+      <c r="B25" s="32" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="17">
+      <c r="C25" s="32">
         <v>1.6</v>
       </c>
-      <c r="D25" s="17">
+      <c r="D25" s="32">
         <v>148</v>
       </c>
-      <c r="E25" s="17">
+      <c r="E25" s="32">
         <v>111</v>
       </c>
-      <c r="F25" s="17">
+      <c r="F25" s="32">
         <v>185</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15.75" thickBot="1">
+    <row r="26" spans="1:17" ht="15.75" thickBot="1">
       <c r="A26" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="33" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="33">
         <v>0.76</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="33">
         <v>222</v>
       </c>
-      <c r="E26" s="20">
+      <c r="E26" s="33">
         <v>222</v>
       </c>
-      <c r="F26" s="20">
+      <c r="F26" s="33">
         <v>222</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>95</v>
       </c>
     </row>
+    <row r="27" spans="1:17">
+      <c r="B27" s="34"/>
+      <c r="C27" s="34"/>
+      <c r="D27" s="34"/>
+      <c r="E27" s="34"/>
+      <c r="F27" s="34"/>
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27" s="35">
+        <v>5</v>
+      </c>
+      <c r="N27" s="35">
+        <v>9</v>
+      </c>
+      <c r="O27" s="35">
+        <v>11</v>
+      </c>
+      <c r="P27" s="35">
+        <f t="shared" ref="P27:P30" si="0">O27-N27</f>
+        <v>2</v>
+      </c>
+      <c r="Q27" s="5">
+        <f t="shared" ref="Q27:Q30" si="1">2*DEGREES(TANH(((O27-N27)/2/M27)))</f>
+        <v>22.617545657860241</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="L28">
+        <v>1</v>
+      </c>
+      <c r="M28" s="35">
+        <v>2</v>
+      </c>
+      <c r="N28" s="35">
+        <v>-0.5</v>
+      </c>
+      <c r="O28" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="P28" s="35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="Q28" s="5">
+        <f t="shared" si="1"/>
+        <v>28.065611359443928</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="L29">
+        <v>2</v>
+      </c>
+      <c r="M29" s="35">
+        <v>5</v>
+      </c>
+      <c r="N29" s="35">
+        <v>8</v>
+      </c>
+      <c r="O29" s="35">
+        <v>12</v>
+      </c>
+      <c r="P29" s="35">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Q29" s="5">
+        <f t="shared" si="1"/>
+        <v>43.538943935199605</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="L30">
+        <v>2</v>
+      </c>
+      <c r="M30" s="35">
+        <v>3</v>
+      </c>
+      <c r="N30" s="35">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="O30" s="35">
+        <v>11.3</v>
+      </c>
+      <c r="P30" s="35">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="Q30" s="5">
+        <f t="shared" si="1"/>
+        <v>45.162661140351425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="L31">
+        <v>2</v>
+      </c>
+      <c r="M31" s="35">
+        <v>1.5</v>
+      </c>
+      <c r="N31" s="35">
+        <v>-0.7</v>
+      </c>
+      <c r="O31" s="35">
+        <v>0.7</v>
+      </c>
+      <c r="P31" s="35">
+        <f>O31-N31</f>
+        <v>1.4</v>
+      </c>
+      <c r="Q31" s="5">
+        <f>2*DEGREES(TANH(((O31-N31)/2/M31)))</f>
+        <v>49.904866192765191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="L32">
+        <v>5</v>
+      </c>
+      <c r="M32" s="35">
+        <v>4</v>
+      </c>
+      <c r="N32" s="35">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="O32" s="35">
+        <v>11.2</v>
+      </c>
+      <c r="P32" s="35">
+        <f>O32-N32</f>
+        <v>2.3999999999999986</v>
+      </c>
+      <c r="Q32" s="5">
+        <f>2*DEGREES(TANH(((O32-N32)/2/M32)))</f>
+        <v>33.381966424812695</v>
+      </c>
+    </row>
+    <row r="33" spans="12:17">
+      <c r="L33">
+        <v>5</v>
+      </c>
+      <c r="M33" s="35">
+        <v>5</v>
+      </c>
+      <c r="N33" s="35">
+        <v>8.6</v>
+      </c>
+      <c r="O33" s="35">
+        <v>11.6</v>
+      </c>
+      <c r="P33" s="35">
+        <f t="shared" ref="P33:P35" si="2">O33-N33</f>
+        <v>3</v>
+      </c>
+      <c r="Q33" s="5">
+        <f t="shared" ref="Q33:Q35" si="3">2*DEGREES(TANH(((O33-N33)/2/M33)))</f>
+        <v>33.381966424812703</v>
+      </c>
+    </row>
+    <row r="34" spans="12:17">
+      <c r="L34">
+        <v>5</v>
+      </c>
+      <c r="M34" s="35">
+        <v>2</v>
+      </c>
+      <c r="N34" s="35">
+        <v>-0.7</v>
+      </c>
+      <c r="O34" s="35">
+        <v>0.7</v>
+      </c>
+      <c r="P34" s="35">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="Q34" s="5">
+        <f t="shared" si="3"/>
+        <v>38.545798043775079</v>
+      </c>
+    </row>
+    <row r="35" spans="12:17">
+      <c r="L35">
+        <v>4</v>
+      </c>
+      <c r="M35" s="35">
+        <v>5</v>
+      </c>
+      <c r="N35" s="35">
+        <v>8</v>
+      </c>
+      <c r="O35" s="35">
+        <v>11.1</v>
+      </c>
+      <c r="P35" s="35">
+        <f t="shared" si="2"/>
+        <v>3.0999999999999996</v>
+      </c>
+      <c r="Q35" s="5">
+        <f t="shared" si="3"/>
+        <v>34.427555351444965</v>
+      </c>
+    </row>
+    <row r="36" spans="12:17">
+      <c r="L36">
+        <v>7</v>
+      </c>
+      <c r="M36" s="35">
+        <v>5</v>
+      </c>
+      <c r="N36" s="35">
+        <v>7.7</v>
+      </c>
+      <c r="O36" s="35">
+        <v>11.1</v>
+      </c>
+      <c r="P36" s="35">
+        <f t="shared" ref="P36:P45" si="4">O36-N36</f>
+        <v>3.3999999999999995</v>
+      </c>
+      <c r="Q36" s="5">
+        <f t="shared" ref="Q36:Q45" si="5">2*DEGREES(TANH(((O36-N36)/2/M36)))</f>
+        <v>37.52614521695638</v>
+      </c>
+    </row>
+    <row r="37" spans="12:17">
+      <c r="L37">
+        <v>3</v>
+      </c>
+      <c r="M37" s="35">
+        <v>5</v>
+      </c>
+      <c r="N37" s="35">
+        <v>8</v>
+      </c>
+      <c r="O37" s="35">
+        <v>11.6</v>
+      </c>
+      <c r="P37" s="35">
+        <f t="shared" si="4"/>
+        <v>3.5999999999999996</v>
+      </c>
+      <c r="Q37" s="5">
+        <f t="shared" si="5"/>
+        <v>39.558614369300948</v>
+      </c>
+    </row>
+    <row r="38" spans="12:17">
+      <c r="L38">
+        <v>3</v>
+      </c>
+      <c r="M38" s="35">
+        <v>3</v>
+      </c>
+      <c r="N38" s="35">
+        <v>-0.1</v>
+      </c>
+      <c r="O38" s="35">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P38" s="35">
+        <f t="shared" si="4"/>
+        <v>2.3000000000000003</v>
+      </c>
+      <c r="Q38" s="5">
+        <f t="shared" si="5"/>
+        <v>41.894533282939882</v>
+      </c>
+    </row>
+    <row r="39" spans="12:17">
+      <c r="L39">
+        <v>6</v>
+      </c>
+      <c r="M39" s="35">
+        <v>5</v>
+      </c>
+      <c r="N39" s="35">
+        <v>-0.8</v>
+      </c>
+      <c r="O39" s="35">
+        <v>2.6</v>
+      </c>
+      <c r="P39" s="35">
+        <f t="shared" si="4"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="Q39" s="5">
+        <f t="shared" si="5"/>
+        <v>37.526145216956387</v>
+      </c>
+    </row>
+    <row r="40" spans="12:17">
+      <c r="L40">
+        <v>9</v>
+      </c>
+      <c r="M40" s="35">
+        <v>5</v>
+      </c>
+      <c r="N40" s="35">
+        <v>7.5</v>
+      </c>
+      <c r="O40" s="35">
+        <v>10.9</v>
+      </c>
+      <c r="P40" s="35">
+        <f t="shared" si="4"/>
+        <v>3.4000000000000004</v>
+      </c>
+      <c r="Q40" s="5">
+        <f t="shared" si="5"/>
+        <v>37.526145216956387</v>
+      </c>
+    </row>
+    <row r="41" spans="12:17">
+      <c r="L41">
+        <v>8</v>
+      </c>
+      <c r="M41" s="35">
+        <v>5</v>
+      </c>
+      <c r="N41" s="35">
+        <v>8.4</v>
+      </c>
+      <c r="O41" s="35">
+        <v>11.7</v>
+      </c>
+      <c r="P41" s="35">
+        <f t="shared" si="4"/>
+        <v>3.2999999999999989</v>
+      </c>
+      <c r="Q41" s="5">
+        <f t="shared" si="5"/>
+        <v>36.499792407513674</v>
+      </c>
+    </row>
+    <row r="42" spans="12:17">
+      <c r="M42" s="35"/>
+      <c r="N42" s="35"/>
+      <c r="O42" s="35"/>
+      <c r="P42" s="35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q42" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="43" spans="12:17">
+      <c r="M43" s="35"/>
+      <c r="N43" s="35"/>
+      <c r="O43" s="35"/>
+      <c r="P43" s="35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q43" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="44" spans="12:17">
+      <c r="M44" s="35"/>
+      <c r="N44" s="35"/>
+      <c r="O44" s="35"/>
+      <c r="P44" s="35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q44" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="45" spans="12:17">
+      <c r="P45" s="35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q45" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A5:K26"/>
   <mergeCells count="4">
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="D1:F1"/>
@@ -2282,7 +2719,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
All works: Arduino can scan a barcode, send it to both Windows ad Azure Job. On Azure, it will convert to Jpeg and recognize barcode.
</commit_message>
<xml_diff>
--- a/Docs/Camera module overview.xlsx
+++ b/Docs/Camera module overview.xlsx
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="130">
   <si>
     <t>Technical specs comparison</t>
   </si>
@@ -527,6 +527,12 @@
   </si>
   <si>
     <t>view width</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/CCTV-Camera-Lens-78-Degree-F1-8-FIXED-IRIS-1-2-5-IR-300-MegaPixel-M12/32744411682.html?spm=a2g0s.9042311.0.0.ZaCeBU</t>
+  </si>
+  <si>
+    <t>https://www.aliexpress.com/item/Yumiki-3-0Megpixel-M12-MTV-6mm-3MP-HD-CCTV-Camera-Lens-IR-HD-Security-Camera-Lens/32791613452.html?spm=a2g0s.9042311.0.0.ZaCeBU</t>
   </si>
 </sst>
 </file>
@@ -686,7 +692,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -749,15 +755,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -767,6 +764,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -1706,10 +1714,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Q45"/>
+  <dimension ref="A1:R45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1723,7 +1731,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="33" t="s">
         <v>63</v>
       </c>
       <c r="B1" s="17" t="s">
@@ -1732,32 +1740,32 @@
       <c r="C1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="33" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29" t="s">
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="30"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="16" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31"/>
-      <c r="G2" s="30"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="34"/>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="30"/>
+      <c r="A3" s="34"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
@@ -1769,10 +1777,10 @@
       <c r="F3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="30"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:17" ht="43.5" thickBot="1">
-      <c r="A4" s="31"/>
+      <c r="A4" s="35"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16" t="s">
@@ -1784,7 +1792,7 @@
       <c r="F4" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="31"/>
+      <c r="G4" s="35"/>
       <c r="I4" s="16" t="s">
         <v>103</v>
       </c>
@@ -1814,19 +1822,19 @@
       <c r="A5" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C5" s="32">
+      <c r="C5" s="29">
         <v>3.2</v>
       </c>
-      <c r="D5" s="32">
+      <c r="D5" s="29">
         <v>68</v>
       </c>
-      <c r="E5" s="32">
+      <c r="E5" s="29">
         <v>51</v>
       </c>
-      <c r="F5" s="32">
+      <c r="F5" s="29">
         <v>85</v>
       </c>
       <c r="G5" s="17"/>
@@ -1835,19 +1843,19 @@
       <c r="A6" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="32">
+      <c r="C6" s="29">
         <v>2.8</v>
       </c>
-      <c r="D6" s="32">
+      <c r="D6" s="29">
         <v>90</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="29">
         <v>68</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="29">
         <v>112</v>
       </c>
       <c r="G6" s="17"/>
@@ -1856,19 +1864,19 @@
       <c r="A7" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C7" s="32">
+      <c r="C7" s="29">
         <v>2.6</v>
       </c>
-      <c r="D7" s="32">
+      <c r="D7" s="29">
         <v>90</v>
       </c>
-      <c r="E7" s="32">
+      <c r="E7" s="29">
         <v>68</v>
       </c>
-      <c r="F7" s="32">
+      <c r="F7" s="29">
         <v>112</v>
       </c>
       <c r="G7" s="17"/>
@@ -1884,19 +1892,19 @@
       <c r="A8" s="18" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="32" t="s">
+      <c r="B8" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C8" s="32">
+      <c r="C8" s="29">
         <v>2.8</v>
       </c>
-      <c r="D8" s="32">
+      <c r="D8" s="29">
         <v>90</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="29">
         <v>68</v>
       </c>
-      <c r="F8" s="32">
+      <c r="F8" s="29">
         <v>112</v>
       </c>
       <c r="G8" s="17"/>
@@ -1905,19 +1913,19 @@
       <c r="A9" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="32">
+      <c r="C9" s="29">
         <v>1.8</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="29">
         <v>104</v>
       </c>
-      <c r="E9" s="32">
+      <c r="E9" s="29">
         <v>78</v>
       </c>
-      <c r="F9" s="32">
+      <c r="F9" s="29">
         <v>130</v>
       </c>
       <c r="G9" s="17"/>
@@ -1926,19 +1934,19 @@
       <c r="A10" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="29">
         <v>6</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="29">
         <v>48</v>
       </c>
-      <c r="E10" s="32">
+      <c r="E10" s="29">
         <v>36</v>
       </c>
-      <c r="F10" s="32">
+      <c r="F10" s="29">
         <v>60</v>
       </c>
       <c r="G10" s="17"/>
@@ -1947,19 +1955,19 @@
       <c r="A11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="32">
+      <c r="C11" s="29">
         <v>8</v>
       </c>
-      <c r="D11" s="32">
+      <c r="D11" s="29">
         <v>36</v>
       </c>
-      <c r="E11" s="32">
+      <c r="E11" s="29">
         <v>27</v>
       </c>
-      <c r="F11" s="32">
+      <c r="F11" s="29">
         <v>45</v>
       </c>
       <c r="G11" s="17"/>
@@ -1968,19 +1976,19 @@
       <c r="A12" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="32">
+      <c r="C12" s="29">
         <v>12</v>
       </c>
-      <c r="D12" s="32">
+      <c r="D12" s="29">
         <v>20</v>
       </c>
-      <c r="E12" s="32">
+      <c r="E12" s="29">
         <v>15</v>
       </c>
-      <c r="F12" s="32">
+      <c r="F12" s="29">
         <v>25</v>
       </c>
       <c r="G12" s="17"/>
@@ -1989,19 +1997,19 @@
       <c r="A13" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="32">
+      <c r="C13" s="29">
         <v>10</v>
       </c>
-      <c r="D13" s="32">
+      <c r="D13" s="29">
         <v>18</v>
       </c>
-      <c r="E13" s="32">
+      <c r="E13" s="29">
         <v>13</v>
       </c>
-      <c r="F13" s="32">
+      <c r="F13" s="29">
         <v>22</v>
       </c>
       <c r="G13" s="17"/>
@@ -2010,19 +2018,19 @@
       <c r="A14" s="18" t="s">
         <v>82</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="32">
+      <c r="C14" s="29">
         <v>2.8</v>
       </c>
-      <c r="D14" s="32">
+      <c r="D14" s="29">
         <v>96</v>
       </c>
-      <c r="E14" s="32">
+      <c r="E14" s="29">
         <v>72</v>
       </c>
-      <c r="F14" s="32">
+      <c r="F14" s="29">
         <v>120</v>
       </c>
       <c r="G14" s="17"/>
@@ -2031,19 +2039,19 @@
       <c r="A15" s="18" t="s">
         <v>83</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="32">
+      <c r="C15" s="29">
         <v>2.1</v>
       </c>
-      <c r="D15" s="32">
+      <c r="D15" s="29">
         <v>116</v>
       </c>
-      <c r="E15" s="32">
+      <c r="E15" s="29">
         <v>87</v>
       </c>
-      <c r="F15" s="32">
+      <c r="F15" s="29">
         <v>145</v>
       </c>
       <c r="G15" s="17"/>
@@ -2052,262 +2060,262 @@
       <c r="A16" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16" s="29">
         <v>2.25</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16" s="29">
         <v>136</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16" s="29">
         <v>102</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16" s="29">
         <v>170</v>
       </c>
       <c r="G16" s="17"/>
     </row>
-    <row r="17" spans="1:17" ht="15.75" thickBot="1">
+    <row r="17" spans="1:18" ht="15.75" thickBot="1">
       <c r="A17" s="18" t="s">
         <v>85</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="29" t="s">
         <v>86</v>
       </c>
-      <c r="C17" s="32">
+      <c r="C17" s="29">
         <v>4</v>
       </c>
-      <c r="D17" s="32">
+      <c r="D17" s="29">
         <v>84</v>
       </c>
-      <c r="E17" s="32">
+      <c r="E17" s="29">
         <v>63</v>
       </c>
-      <c r="F17" s="32">
+      <c r="F17" s="29">
         <v>105</v>
       </c>
       <c r="G17" s="17"/>
     </row>
-    <row r="18" spans="1:17" ht="15.75" thickBot="1">
+    <row r="18" spans="1:18" ht="15.75" thickBot="1">
       <c r="A18" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C18" s="32">
+      <c r="C18" s="29">
         <v>3.8</v>
       </c>
-      <c r="D18" s="32">
+      <c r="D18" s="29">
         <v>85</v>
       </c>
-      <c r="E18" s="32">
+      <c r="E18" s="29">
         <v>64</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="29">
         <v>106</v>
       </c>
       <c r="G18" s="17"/>
     </row>
-    <row r="19" spans="1:17" ht="15.75" thickBot="1">
+    <row r="19" spans="1:18" ht="15.75" thickBot="1">
       <c r="A19" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="29">
         <v>2.8</v>
       </c>
-      <c r="D19" s="32">
+      <c r="D19" s="29">
         <v>110</v>
       </c>
-      <c r="E19" s="32">
+      <c r="E19" s="29">
         <v>83</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F19" s="29">
         <v>138</v>
       </c>
       <c r="G19" s="17"/>
     </row>
-    <row r="20" spans="1:17" ht="15.75" thickBot="1">
+    <row r="20" spans="1:18" ht="15.75" thickBot="1">
       <c r="A20" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C20" s="32">
+      <c r="C20" s="29">
         <v>3</v>
       </c>
-      <c r="D20" s="32">
+      <c r="D20" s="29">
         <v>112</v>
       </c>
-      <c r="E20" s="32">
+      <c r="E20" s="29">
         <v>84</v>
       </c>
-      <c r="F20" s="32">
+      <c r="F20" s="29">
         <v>140</v>
       </c>
       <c r="G20" s="17"/>
     </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1">
+    <row r="21" spans="1:18" ht="15.75" thickBot="1">
       <c r="A21" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="29" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="32">
+      <c r="C21" s="29">
         <v>2.8</v>
       </c>
-      <c r="D21" s="32">
+      <c r="D21" s="29">
         <v>124</v>
       </c>
-      <c r="E21" s="32">
+      <c r="E21" s="29">
         <v>93</v>
       </c>
-      <c r="F21" s="32">
+      <c r="F21" s="29">
         <v>155</v>
       </c>
       <c r="G21" s="17"/>
     </row>
-    <row r="22" spans="1:17" ht="15.75" thickBot="1">
+    <row r="22" spans="1:18" ht="15.75" thickBot="1">
       <c r="A22" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C22" s="32">
+      <c r="C22" s="29">
         <v>1.56</v>
       </c>
-      <c r="D22" s="32">
+      <c r="D22" s="29">
         <v>191</v>
       </c>
-      <c r="E22" s="32">
+      <c r="E22" s="29">
         <v>127</v>
       </c>
-      <c r="F22" s="32">
+      <c r="F22" s="29">
         <v>204</v>
       </c>
       <c r="G22" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15.75" thickBot="1">
+    <row r="23" spans="1:18" ht="15.75" thickBot="1">
       <c r="A23" s="18" t="s">
         <v>96</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="C23" s="32">
+      <c r="C23" s="29">
         <v>1.05</v>
       </c>
-      <c r="D23" s="32">
+      <c r="D23" s="29">
         <v>194</v>
       </c>
-      <c r="E23" s="32">
+      <c r="E23" s="29">
         <v>142</v>
       </c>
-      <c r="F23" s="32">
+      <c r="F23" s="29">
         <v>206</v>
       </c>
       <c r="G23" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15.75" thickBot="1">
+    <row r="24" spans="1:18" ht="15.75" thickBot="1">
       <c r="A24" s="18" t="s">
         <v>97</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="C24" s="32">
+      <c r="C24" s="29">
         <v>1.58</v>
       </c>
-      <c r="D24" s="32">
+      <c r="D24" s="29">
         <v>185</v>
       </c>
-      <c r="E24" s="32">
+      <c r="E24" s="29">
         <v>139</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="29">
         <v>200</v>
       </c>
       <c r="G24" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15.75" thickBot="1">
+    <row r="25" spans="1:18" ht="15.75" thickBot="1">
       <c r="A25" s="18" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="32" t="s">
+      <c r="B25" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="32">
+      <c r="C25" s="29">
         <v>1.6</v>
       </c>
-      <c r="D25" s="32">
+      <c r="D25" s="29">
         <v>148</v>
       </c>
-      <c r="E25" s="32">
+      <c r="E25" s="29">
         <v>111</v>
       </c>
-      <c r="F25" s="32">
+      <c r="F25" s="29">
         <v>185</v>
       </c>
       <c r="G25" s="17" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" thickBot="1">
+    <row r="26" spans="1:18" ht="15.75" thickBot="1">
       <c r="A26" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B26" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="33">
+      <c r="C26" s="30">
         <v>0.76</v>
       </c>
-      <c r="D26" s="33">
+      <c r="D26" s="30">
         <v>222</v>
       </c>
-      <c r="E26" s="33">
+      <c r="E26" s="30">
         <v>222</v>
       </c>
-      <c r="F26" s="33">
+      <c r="F26" s="30">
         <v>222</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
+    <row r="27" spans="1:18">
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
       <c r="L27">
         <v>1</v>
       </c>
-      <c r="M27" s="35">
+      <c r="M27" s="32">
         <v>5</v>
       </c>
-      <c r="N27" s="35">
+      <c r="N27" s="32">
         <v>9</v>
       </c>
-      <c r="O27" s="35">
+      <c r="O27" s="32">
         <v>11</v>
       </c>
-      <c r="P27" s="35">
+      <c r="P27" s="32">
         <f t="shared" ref="P27:P30" si="0">O27-N27</f>
         <v>2</v>
       </c>
@@ -2315,26 +2323,29 @@
         <f t="shared" ref="Q27:Q30" si="1">2*DEGREES(TANH(((O27-N27)/2/M27)))</f>
         <v>22.617545657860241</v>
       </c>
-    </row>
-    <row r="28" spans="1:17">
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
+      <c r="R27" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" thickBot="1">
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
       <c r="L28">
         <v>1</v>
       </c>
-      <c r="M28" s="35">
+      <c r="M28" s="32">
         <v>2</v>
       </c>
-      <c r="N28" s="35">
+      <c r="N28" s="32">
         <v>-0.5</v>
       </c>
-      <c r="O28" s="35">
+      <c r="O28" s="32">
         <v>0.5</v>
       </c>
-      <c r="P28" s="35">
+      <c r="P28" s="32">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
@@ -2342,87 +2353,94 @@
         <f t="shared" si="1"/>
         <v>28.065611359443928</v>
       </c>
-    </row>
-    <row r="29" spans="1:17">
-      <c r="L29">
+      <c r="R28" s="1"/>
+    </row>
+    <row r="29" spans="1:18">
+      <c r="B29" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="29">
+        <v>2.8</v>
+      </c>
+      <c r="L29" s="21">
         <v>2</v>
       </c>
-      <c r="M29" s="35">
+      <c r="M29" s="36">
         <v>5</v>
       </c>
-      <c r="N29" s="35">
+      <c r="N29" s="36">
         <v>8</v>
       </c>
-      <c r="O29" s="35">
+      <c r="O29" s="36">
         <v>12</v>
       </c>
-      <c r="P29" s="35">
+      <c r="P29" s="36">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="Q29" s="5">
+      <c r="Q29" s="37">
         <f t="shared" si="1"/>
         <v>43.538943935199605</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
-      <c r="L30">
+    <row r="30" spans="1:18">
+      <c r="L30" s="21">
         <v>2</v>
       </c>
-      <c r="M30" s="35">
+      <c r="M30" s="36">
         <v>3</v>
       </c>
-      <c r="N30" s="35">
+      <c r="N30" s="36">
         <v>8.8000000000000007</v>
       </c>
-      <c r="O30" s="35">
+      <c r="O30" s="36">
         <v>11.3</v>
       </c>
-      <c r="P30" s="35">
+      <c r="P30" s="36">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="Q30" s="5">
+      <c r="Q30" s="37">
         <f t="shared" si="1"/>
         <v>45.162661140351425</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
-      <c r="L31">
+    <row r="31" spans="1:18">
+      <c r="L31" s="21">
         <v>2</v>
       </c>
-      <c r="M31" s="35">
+      <c r="M31" s="36">
         <v>1.5</v>
       </c>
-      <c r="N31" s="35">
+      <c r="N31" s="36">
         <v>-0.7</v>
       </c>
-      <c r="O31" s="35">
+      <c r="O31" s="36">
         <v>0.7</v>
       </c>
-      <c r="P31" s="35">
+      <c r="P31" s="36">
         <f>O31-N31</f>
         <v>1.4</v>
       </c>
-      <c r="Q31" s="5">
+      <c r="Q31" s="37">
         <f>2*DEGREES(TANH(((O31-N31)/2/M31)))</f>
         <v>49.904866192765191</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:18">
       <c r="L32">
         <v>5</v>
       </c>
-      <c r="M32" s="35">
+      <c r="M32" s="32">
         <v>4</v>
       </c>
-      <c r="N32" s="35">
+      <c r="N32" s="32">
         <v>8.8000000000000007</v>
       </c>
-      <c r="O32" s="35">
+      <c r="O32" s="32">
         <v>11.2</v>
       </c>
-      <c r="P32" s="35">
+      <c r="P32" s="32">
         <f>O32-N32</f>
         <v>2.3999999999999986</v>
       </c>
@@ -2431,20 +2449,20 @@
         <v>33.381966424812695</v>
       </c>
     </row>
-    <row r="33" spans="12:17">
+    <row r="33" spans="12:18">
       <c r="L33">
         <v>5</v>
       </c>
-      <c r="M33" s="35">
+      <c r="M33" s="32">
         <v>5</v>
       </c>
-      <c r="N33" s="35">
+      <c r="N33" s="32">
         <v>8.6</v>
       </c>
-      <c r="O33" s="35">
+      <c r="O33" s="32">
         <v>11.6</v>
       </c>
-      <c r="P33" s="35">
+      <c r="P33" s="32">
         <f t="shared" ref="P33:P35" si="2">O33-N33</f>
         <v>3</v>
       </c>
@@ -2453,20 +2471,20 @@
         <v>33.381966424812703</v>
       </c>
     </row>
-    <row r="34" spans="12:17">
+    <row r="34" spans="12:18">
       <c r="L34">
         <v>5</v>
       </c>
-      <c r="M34" s="35">
+      <c r="M34" s="32">
         <v>2</v>
       </c>
-      <c r="N34" s="35">
+      <c r="N34" s="32">
         <v>-0.7</v>
       </c>
-      <c r="O34" s="35">
+      <c r="O34" s="32">
         <v>0.7</v>
       </c>
-      <c r="P34" s="35">
+      <c r="P34" s="32">
         <f t="shared" si="2"/>
         <v>1.4</v>
       </c>
@@ -2475,20 +2493,20 @@
         <v>38.545798043775079</v>
       </c>
     </row>
-    <row r="35" spans="12:17">
+    <row r="35" spans="12:18">
       <c r="L35">
         <v>4</v>
       </c>
-      <c r="M35" s="35">
+      <c r="M35" s="32">
         <v>5</v>
       </c>
-      <c r="N35" s="35">
+      <c r="N35" s="32">
         <v>8</v>
       </c>
-      <c r="O35" s="35">
+      <c r="O35" s="32">
         <v>11.1</v>
       </c>
-      <c r="P35" s="35">
+      <c r="P35" s="32">
         <f t="shared" si="2"/>
         <v>3.0999999999999996</v>
       </c>
@@ -2496,21 +2514,24 @@
         <f t="shared" si="3"/>
         <v>34.427555351444965</v>
       </c>
-    </row>
-    <row r="36" spans="12:17">
+      <c r="R35" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="36" spans="12:18">
       <c r="L36">
         <v>7</v>
       </c>
-      <c r="M36" s="35">
+      <c r="M36" s="32">
         <v>5</v>
       </c>
-      <c r="N36" s="35">
+      <c r="N36" s="32">
         <v>7.7</v>
       </c>
-      <c r="O36" s="35">
+      <c r="O36" s="32">
         <v>11.1</v>
       </c>
-      <c r="P36" s="35">
+      <c r="P36" s="32">
         <f t="shared" ref="P36:P45" si="4">O36-N36</f>
         <v>3.3999999999999995</v>
       </c>
@@ -2518,21 +2539,22 @@
         <f t="shared" ref="Q36:Q45" si="5">2*DEGREES(TANH(((O36-N36)/2/M36)))</f>
         <v>37.52614521695638</v>
       </c>
-    </row>
-    <row r="37" spans="12:17">
+      <c r="R36" s="1"/>
+    </row>
+    <row r="37" spans="12:18">
       <c r="L37">
         <v>3</v>
       </c>
-      <c r="M37" s="35">
+      <c r="M37" s="32">
         <v>5</v>
       </c>
-      <c r="N37" s="35">
+      <c r="N37" s="32">
         <v>8</v>
       </c>
-      <c r="O37" s="35">
+      <c r="O37" s="32">
         <v>11.6</v>
       </c>
-      <c r="P37" s="35">
+      <c r="P37" s="32">
         <f t="shared" si="4"/>
         <v>3.5999999999999996</v>
       </c>
@@ -2541,20 +2563,20 @@
         <v>39.558614369300948</v>
       </c>
     </row>
-    <row r="38" spans="12:17">
+    <row r="38" spans="12:18">
       <c r="L38">
         <v>3</v>
       </c>
-      <c r="M38" s="35">
+      <c r="M38" s="32">
         <v>3</v>
       </c>
-      <c r="N38" s="35">
+      <c r="N38" s="32">
         <v>-0.1</v>
       </c>
-      <c r="O38" s="35">
+      <c r="O38" s="32">
         <v>2.2000000000000002</v>
       </c>
-      <c r="P38" s="35">
+      <c r="P38" s="32">
         <f t="shared" si="4"/>
         <v>2.3000000000000003</v>
       </c>
@@ -2563,20 +2585,20 @@
         <v>41.894533282939882</v>
       </c>
     </row>
-    <row r="39" spans="12:17">
+    <row r="39" spans="12:18">
       <c r="L39">
         <v>6</v>
       </c>
-      <c r="M39" s="35">
+      <c r="M39" s="32">
         <v>5</v>
       </c>
-      <c r="N39" s="35">
+      <c r="N39" s="32">
         <v>-0.8</v>
       </c>
-      <c r="O39" s="35">
+      <c r="O39" s="32">
         <v>2.6</v>
       </c>
-      <c r="P39" s="35">
+      <c r="P39" s="32">
         <f t="shared" si="4"/>
         <v>3.4000000000000004</v>
       </c>
@@ -2585,20 +2607,20 @@
         <v>37.526145216956387</v>
       </c>
     </row>
-    <row r="40" spans="12:17">
+    <row r="40" spans="12:18">
       <c r="L40">
         <v>9</v>
       </c>
-      <c r="M40" s="35">
+      <c r="M40" s="32">
         <v>5</v>
       </c>
-      <c r="N40" s="35">
+      <c r="N40" s="32">
         <v>7.5</v>
       </c>
-      <c r="O40" s="35">
+      <c r="O40" s="32">
         <v>10.9</v>
       </c>
-      <c r="P40" s="35">
+      <c r="P40" s="32">
         <f t="shared" si="4"/>
         <v>3.4000000000000004</v>
       </c>
@@ -2607,20 +2629,20 @@
         <v>37.526145216956387</v>
       </c>
     </row>
-    <row r="41" spans="12:17">
+    <row r="41" spans="12:18">
       <c r="L41">
         <v>8</v>
       </c>
-      <c r="M41" s="35">
+      <c r="M41" s="32">
         <v>5</v>
       </c>
-      <c r="N41" s="35">
+      <c r="N41" s="32">
         <v>8.4</v>
       </c>
-      <c r="O41" s="35">
+      <c r="O41" s="32">
         <v>11.7</v>
       </c>
-      <c r="P41" s="35">
+      <c r="P41" s="32">
         <f t="shared" si="4"/>
         <v>3.2999999999999989</v>
       </c>
@@ -2629,11 +2651,11 @@
         <v>36.499792407513674</v>
       </c>
     </row>
-    <row r="42" spans="12:17">
-      <c r="M42" s="35"/>
-      <c r="N42" s="35"/>
-      <c r="O42" s="35"/>
-      <c r="P42" s="35">
+    <row r="42" spans="12:18">
+      <c r="M42" s="32"/>
+      <c r="N42" s="32"/>
+      <c r="O42" s="32"/>
+      <c r="P42" s="32">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2642,11 +2664,11 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="43" spans="12:17">
-      <c r="M43" s="35"/>
-      <c r="N43" s="35"/>
-      <c r="O43" s="35"/>
-      <c r="P43" s="35">
+    <row r="43" spans="12:18">
+      <c r="M43" s="32"/>
+      <c r="N43" s="32"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="32">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2655,11 +2677,11 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="44" spans="12:17">
-      <c r="M44" s="35"/>
-      <c r="N44" s="35"/>
-      <c r="O44" s="35"/>
-      <c r="P44" s="35">
+    <row r="44" spans="12:18">
+      <c r="M44" s="32"/>
+      <c r="N44" s="32"/>
+      <c r="O44" s="32"/>
+      <c r="P44" s="32">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2668,8 +2690,8 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="45" spans="12:17">
-      <c r="P45" s="35">
+    <row r="45" spans="12:18">
+      <c r="P45" s="32">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -2709,6 +2731,8 @@
     <hyperlink ref="A24" r:id="rId20" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS-30180.jpg"/>
     <hyperlink ref="A25" r:id="rId21" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS25180.JPG"/>
     <hyperlink ref="A26" r:id="rId22" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS-32220.pdf"/>
+    <hyperlink ref="R35" r:id="rId23"/>
+    <hyperlink ref="R27" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2720,7 +2744,7 @@
   <dimension ref="A2:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2744,7 +2768,7 @@
         <v>40</v>
       </c>
       <c r="B3" s="6">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
         <v>54</v>
@@ -2757,7 +2781,7 @@
         <v>41</v>
       </c>
       <c r="B4" s="6">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
         <v>55</v>
@@ -2771,7 +2795,7 @@
       </c>
       <c r="B5" s="5">
         <f>2*SINH(obj_width/2/MOD)/(2*PI())*360</f>
-        <v>86.927289045631397</v>
+        <v>157.88220923994655</v>
       </c>
       <c r="C5" t="s">
         <v>45</v>
@@ -2822,7 +2846,7 @@
       </c>
       <c r="B9" s="5">
         <f>FOV</f>
-        <v>86.927289045631397</v>
+        <v>157.88220923994655</v>
       </c>
       <c r="C9" t="s">
         <v>49</v>
@@ -2836,7 +2860,7 @@
       </c>
       <c r="B10" s="5">
         <f>FOV*B8</f>
-        <v>115.90305206084187</v>
+        <v>210.50961231992875</v>
       </c>
       <c r="C10" t="s">
         <v>48</v>
@@ -2850,7 +2874,7 @@
       </c>
       <c r="B11" s="5">
         <f>SQRT(1+aspect*aspect)*FOV</f>
-        <v>144.87881507605235</v>
+        <v>263.13701539991092</v>
       </c>
       <c r="C11" t="s">
         <v>50</v>
@@ -2864,7 +2888,7 @@
       </c>
       <c r="B12" s="21">
         <f>d*(ccd_h/H)</f>
-        <v>1.7142857142857144</v>
+        <v>1.0666666666666667</v>
       </c>
       <c r="C12" t="s">
         <v>58</v>

</xml_diff>

<commit_message>
Added SimulatedDevice simulating the Arduino as Azure Client. Used to test interface to Azure.
</commit_message>
<xml_diff>
--- a/Docs/Camera module overview.xlsx
+++ b/Docs/Camera module overview.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19001"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21001"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81D65B1-4F7E-480D-86B0-09606AB0C03D}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Camera sensor" sheetId="1" r:id="rId1"/>
@@ -27,17 +28,24 @@
     <definedName name="VFOV">Calculation!$B$9</definedName>
     <definedName name="w">Calculation!$B$6</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>Forfatter</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A16" authorId="0" shapeId="0">
+    <comment ref="A16" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="131">
   <si>
     <t>Technical specs comparison</t>
   </si>
@@ -514,9 +522,6 @@
     <t>Lense #</t>
   </si>
   <si>
-    <t>afstand cm</t>
-  </si>
-  <si>
     <t>left cm</t>
   </si>
   <si>
@@ -533,12 +538,18 @@
   </si>
   <si>
     <t>https://www.aliexpress.com/item/Yumiki-3-0Megpixel-M12-MTV-6mm-3MP-HD-CCTV-Camera-Lens-IR-HD-Security-Camera-Lens/32791613452.html?spm=a2g0s.9042311.0.0.ZaCeBU</t>
+  </si>
+  <si>
+    <t>afstand fra linse cm</t>
+  </si>
+  <si>
+    <t>Afstand fra bund af kamera print</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -764,6 +775,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -773,11 +786,9 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1022,9 +1033,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Kontor">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1062,7 +1073,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Kontor">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1168,7 +1179,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Kontor">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1341,7 +1352,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:W31"/>
   <sheetViews>
@@ -1349,7 +1360,7 @@
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
+      <selection pane="bottomRight" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1698,11 +1709,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J6" r:id="rId1"/>
-    <hyperlink ref="K9" r:id="rId2"/>
-    <hyperlink ref="M5" r:id="rId3"/>
-    <hyperlink ref="M6" r:id="rId4"/>
-    <hyperlink ref="A28" r:id="rId5"/>
+    <hyperlink ref="J6" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="K9" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="M6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="A28" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
@@ -1712,12 +1723,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:R45"/>
+  <dimension ref="A1:R46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="R28" sqref="R28"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="R32" sqref="R32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1728,10 +1739,12 @@
     <col min="4" max="6" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18.42578125" customWidth="1"/>
+    <col min="12" max="16" width="10.42578125" customWidth="1"/>
+    <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="33" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="35" t="s">
         <v>63</v>
       </c>
       <c r="B1" s="17" t="s">
@@ -1740,32 +1753,32 @@
       <c r="C1" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="33" t="s">
+      <c r="D1" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33" t="s">
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15.75" thickBot="1">
-      <c r="A2" s="34"/>
+    <row r="2" spans="1:18" ht="15.75" thickBot="1">
+      <c r="A2" s="36"/>
       <c r="B2" s="16" t="s">
         <v>64</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="34"/>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" s="34"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="36"/>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" s="36"/>
       <c r="B3" s="16"/>
       <c r="C3" s="16"/>
       <c r="D3" s="17" t="s">
@@ -1777,10 +1790,10 @@
       <c r="F3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="34"/>
-    </row>
-    <row r="4" spans="1:17" ht="43.5" thickBot="1">
-      <c r="A4" s="35"/>
+      <c r="G3" s="36"/>
+    </row>
+    <row r="4" spans="1:18" ht="75.75" thickBot="1">
+      <c r="A4" s="37"/>
       <c r="B4" s="16"/>
       <c r="C4" s="16"/>
       <c r="D4" s="16" t="s">
@@ -1792,33 +1805,36 @@
       <c r="F4" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G4" s="35"/>
+      <c r="G4" s="37"/>
       <c r="I4" s="16" t="s">
         <v>103</v>
       </c>
       <c r="K4" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="L4" t="s">
+      <c r="L4" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="P4" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1">
+      <c r="R4" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" thickBot="1">
       <c r="A5" s="18" t="s">
         <v>71</v>
       </c>
@@ -1839,7 +1855,7 @@
       </c>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="1:17" ht="15.75" thickBot="1">
+    <row r="6" spans="1:18" ht="15.75" thickBot="1">
       <c r="A6" s="18" t="s">
         <v>73</v>
       </c>
@@ -1860,7 +1876,7 @@
       </c>
       <c r="G6" s="17"/>
     </row>
-    <row r="7" spans="1:17" ht="15.75" thickBot="1">
+    <row r="7" spans="1:18" ht="15.75" thickBot="1">
       <c r="A7" s="18" t="s">
         <v>74</v>
       </c>
@@ -1888,7 +1904,7 @@
         <v>3.5135135135135136</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15.75" thickBot="1">
+    <row r="8" spans="1:18" ht="15.75" thickBot="1">
       <c r="A8" s="18" t="s">
         <v>75</v>
       </c>
@@ -1909,7 +1925,7 @@
       </c>
       <c r="G8" s="17"/>
     </row>
-    <row r="9" spans="1:17" ht="15.75" thickBot="1">
+    <row r="9" spans="1:18" ht="15.75" thickBot="1">
       <c r="A9" s="18" t="s">
         <v>76</v>
       </c>
@@ -1930,7 +1946,7 @@
       </c>
       <c r="G9" s="17"/>
     </row>
-    <row r="10" spans="1:17" ht="15.75" thickBot="1">
+    <row r="10" spans="1:18" ht="15.75" thickBot="1">
       <c r="A10" s="18" t="s">
         <v>77</v>
       </c>
@@ -1951,7 +1967,7 @@
       </c>
       <c r="G10" s="17"/>
     </row>
-    <row r="11" spans="1:17" ht="15.75" thickBot="1">
+    <row r="11" spans="1:18" ht="15.75" thickBot="1">
       <c r="A11" s="18" t="s">
         <v>79</v>
       </c>
@@ -1972,7 +1988,7 @@
       </c>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:17" ht="15.75" thickBot="1">
+    <row r="12" spans="1:18" ht="15.75" thickBot="1">
       <c r="A12" s="18" t="s">
         <v>80</v>
       </c>
@@ -1993,7 +2009,7 @@
       </c>
       <c r="G12" s="17"/>
     </row>
-    <row r="13" spans="1:17" ht="15.75" thickBot="1">
+    <row r="13" spans="1:18" ht="15.75" thickBot="1">
       <c r="A13" s="18" t="s">
         <v>81</v>
       </c>
@@ -2014,7 +2030,7 @@
       </c>
       <c r="G13" s="17"/>
     </row>
-    <row r="14" spans="1:17" ht="15.75" thickBot="1">
+    <row r="14" spans="1:18" ht="15.75" thickBot="1">
       <c r="A14" s="18" t="s">
         <v>82</v>
       </c>
@@ -2035,7 +2051,7 @@
       </c>
       <c r="G14" s="17"/>
     </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1">
+    <row r="15" spans="1:18" ht="15.75" thickBot="1">
       <c r="A15" s="18" t="s">
         <v>83</v>
       </c>
@@ -2056,7 +2072,7 @@
       </c>
       <c r="G15" s="17"/>
     </row>
-    <row r="16" spans="1:17" ht="15.75" thickBot="1">
+    <row r="16" spans="1:18" ht="15.75" thickBot="1">
       <c r="A16" s="18" t="s">
         <v>84</v>
       </c>
@@ -2324,7 +2340,7 @@
         <v>22.617545657860241</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:18" ht="15.75" thickBot="1">
@@ -2365,20 +2381,20 @@
       <c r="L29" s="21">
         <v>2</v>
       </c>
-      <c r="M29" s="36">
+      <c r="M29" s="33">
         <v>5</v>
       </c>
-      <c r="N29" s="36">
+      <c r="N29" s="33">
         <v>8</v>
       </c>
-      <c r="O29" s="36">
+      <c r="O29" s="33">
         <v>12</v>
       </c>
-      <c r="P29" s="36">
+      <c r="P29" s="33">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="Q29" s="37">
+      <c r="Q29" s="34">
         <f t="shared" si="1"/>
         <v>43.538943935199605</v>
       </c>
@@ -2387,20 +2403,20 @@
       <c r="L30" s="21">
         <v>2</v>
       </c>
-      <c r="M30" s="36">
+      <c r="M30" s="33">
         <v>3</v>
       </c>
-      <c r="N30" s="36">
+      <c r="N30" s="33">
         <v>8.8000000000000007</v>
       </c>
-      <c r="O30" s="36">
+      <c r="O30" s="33">
         <v>11.3</v>
       </c>
-      <c r="P30" s="36">
+      <c r="P30" s="33">
         <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
-      <c r="Q30" s="37">
+      <c r="Q30" s="34">
         <f t="shared" si="1"/>
         <v>45.162661140351425</v>
       </c>
@@ -2409,44 +2425,47 @@
       <c r="L31" s="21">
         <v>2</v>
       </c>
-      <c r="M31" s="36">
+      <c r="M31" s="33">
         <v>1.5</v>
       </c>
-      <c r="N31" s="36">
+      <c r="N31" s="33">
         <v>-0.7</v>
       </c>
-      <c r="O31" s="36">
+      <c r="O31" s="33">
         <v>0.7</v>
       </c>
-      <c r="P31" s="36">
+      <c r="P31" s="33">
         <f>O31-N31</f>
         <v>1.4</v>
       </c>
-      <c r="Q31" s="37">
+      <c r="Q31" s="34">
         <f>2*DEGREES(TANH(((O31-N31)/2/M31)))</f>
         <v>49.904866192765191</v>
       </c>
     </row>
     <row r="32" spans="1:18">
-      <c r="L32">
+      <c r="L32" s="21">
+        <v>2</v>
+      </c>
+      <c r="M32" s="33">
+        <v>6</v>
+      </c>
+      <c r="N32" s="33">
+        <v>0</v>
+      </c>
+      <c r="O32" s="33">
         <v>5</v>
       </c>
-      <c r="M32" s="32">
-        <v>4</v>
-      </c>
-      <c r="N32" s="32">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="O32" s="32">
-        <v>11.2</v>
-      </c>
-      <c r="P32" s="32">
-        <f>O32-N32</f>
-        <v>2.3999999999999986</v>
-      </c>
-      <c r="Q32" s="5">
+      <c r="P32" s="33">
+        <v>5</v>
+      </c>
+      <c r="Q32" s="34">
         <f>2*DEGREES(TANH(((O32-N32)/2/M32)))</f>
-        <v>33.381966424812695</v>
+        <v>45.162661140351425</v>
+      </c>
+      <c r="R32" s="33">
+        <f>P32+2.8</f>
+        <v>7.8</v>
       </c>
     </row>
     <row r="33" spans="12:18">
@@ -2454,21 +2473,21 @@
         <v>5</v>
       </c>
       <c r="M33" s="32">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N33" s="32">
-        <v>8.6</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="O33" s="32">
-        <v>11.6</v>
+        <v>11.2</v>
       </c>
       <c r="P33" s="32">
-        <f t="shared" ref="P33:P35" si="2">O33-N33</f>
-        <v>3</v>
+        <f>O33-N33</f>
+        <v>2.3999999999999986</v>
       </c>
       <c r="Q33" s="5">
-        <f t="shared" ref="Q33:Q35" si="3">2*DEGREES(TANH(((O33-N33)/2/M33)))</f>
-        <v>33.381966424812703</v>
+        <f>2*DEGREES(TANH(((O33-N33)/2/M33)))</f>
+        <v>33.381966424812695</v>
       </c>
     </row>
     <row r="34" spans="12:18">
@@ -2476,149 +2495,149 @@
         <v>5</v>
       </c>
       <c r="M34" s="32">
+        <v>5</v>
+      </c>
+      <c r="N34" s="32">
+        <v>8.6</v>
+      </c>
+      <c r="O34" s="32">
+        <v>11.6</v>
+      </c>
+      <c r="P34" s="32">
+        <f t="shared" ref="P34:P36" si="2">O34-N34</f>
+        <v>3</v>
+      </c>
+      <c r="Q34" s="5">
+        <f t="shared" ref="Q34:Q36" si="3">2*DEGREES(TANH(((O34-N34)/2/M34)))</f>
+        <v>33.381966424812703</v>
+      </c>
+    </row>
+    <row r="35" spans="12:18">
+      <c r="L35">
+        <v>5</v>
+      </c>
+      <c r="M35" s="32">
         <v>2</v>
       </c>
-      <c r="N34" s="32">
+      <c r="N35" s="32">
         <v>-0.7</v>
       </c>
-      <c r="O34" s="32">
+      <c r="O35" s="32">
         <v>0.7</v>
       </c>
-      <c r="P34" s="32">
+      <c r="P35" s="32">
         <f t="shared" si="2"/>
         <v>1.4</v>
       </c>
-      <c r="Q34" s="5">
+      <c r="Q35" s="5">
         <f t="shared" si="3"/>
         <v>38.545798043775079</v>
       </c>
     </row>
-    <row r="35" spans="12:18">
-      <c r="L35">
+    <row r="36" spans="12:18">
+      <c r="L36">
         <v>4</v>
       </c>
-      <c r="M35" s="32">
+      <c r="M36" s="32">
         <v>5</v>
       </c>
-      <c r="N35" s="32">
+      <c r="N36" s="32">
         <v>8</v>
       </c>
-      <c r="O35" s="32">
+      <c r="O36" s="32">
         <v>11.1</v>
       </c>
-      <c r="P35" s="32">
+      <c r="P36" s="32">
         <f t="shared" si="2"/>
         <v>3.0999999999999996</v>
       </c>
-      <c r="Q35" s="5">
+      <c r="Q36" s="5">
         <f t="shared" si="3"/>
         <v>34.427555351444965</v>
       </c>
-      <c r="R35" s="1" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="12:18">
-      <c r="L36">
-        <v>7</v>
-      </c>
-      <c r="M36" s="32">
-        <v>5</v>
-      </c>
-      <c r="N36" s="32">
-        <v>7.7</v>
-      </c>
-      <c r="O36" s="32">
-        <v>11.1</v>
-      </c>
-      <c r="P36" s="32">
-        <f t="shared" ref="P36:P45" si="4">O36-N36</f>
-        <v>3.3999999999999995</v>
-      </c>
-      <c r="Q36" s="5">
-        <f t="shared" ref="Q36:Q45" si="5">2*DEGREES(TANH(((O36-N36)/2/M36)))</f>
-        <v>37.52614521695638</v>
-      </c>
-      <c r="R36" s="1"/>
+      <c r="R36" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="37" spans="12:18">
       <c r="L37">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="M37" s="32">
         <v>5</v>
       </c>
       <c r="N37" s="32">
-        <v>8</v>
+        <v>7.7</v>
       </c>
       <c r="O37" s="32">
-        <v>11.6</v>
+        <v>11.1</v>
       </c>
       <c r="P37" s="32">
-        <f t="shared" si="4"/>
-        <v>3.5999999999999996</v>
+        <f t="shared" ref="P37:P46" si="4">O37-N37</f>
+        <v>3.3999999999999995</v>
       </c>
       <c r="Q37" s="5">
-        <f t="shared" si="5"/>
-        <v>39.558614369300948</v>
-      </c>
+        <f t="shared" ref="Q37:Q46" si="5">2*DEGREES(TANH(((O37-N37)/2/M37)))</f>
+        <v>37.52614521695638</v>
+      </c>
+      <c r="R37" s="1"/>
     </row>
     <row r="38" spans="12:18">
       <c r="L38">
         <v>3</v>
       </c>
       <c r="M38" s="32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="N38" s="32">
-        <v>-0.1</v>
+        <v>8</v>
       </c>
       <c r="O38" s="32">
-        <v>2.2000000000000002</v>
+        <v>11.6</v>
       </c>
       <c r="P38" s="32">
         <f t="shared" si="4"/>
-        <v>2.3000000000000003</v>
+        <v>3.5999999999999996</v>
       </c>
       <c r="Q38" s="5">
         <f t="shared" si="5"/>
-        <v>41.894533282939882</v>
+        <v>39.558614369300948</v>
       </c>
     </row>
     <row r="39" spans="12:18">
       <c r="L39">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="M39" s="32">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N39" s="32">
-        <v>-0.8</v>
+        <v>-0.1</v>
       </c>
       <c r="O39" s="32">
-        <v>2.6</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="P39" s="32">
         <f t="shared" si="4"/>
-        <v>3.4000000000000004</v>
+        <v>2.3000000000000003</v>
       </c>
       <c r="Q39" s="5">
         <f t="shared" si="5"/>
-        <v>37.526145216956387</v>
+        <v>41.894533282939882</v>
       </c>
     </row>
     <row r="40" spans="12:18">
       <c r="L40">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M40" s="32">
         <v>5</v>
       </c>
       <c r="N40" s="32">
-        <v>7.5</v>
+        <v>-0.8</v>
       </c>
       <c r="O40" s="32">
-        <v>10.9</v>
+        <v>2.6</v>
       </c>
       <c r="P40" s="32">
         <f t="shared" si="4"/>
@@ -2631,37 +2650,46 @@
     </row>
     <row r="41" spans="12:18">
       <c r="L41">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M41" s="32">
         <v>5</v>
       </c>
       <c r="N41" s="32">
-        <v>8.4</v>
+        <v>7.5</v>
       </c>
       <c r="O41" s="32">
-        <v>11.7</v>
+        <v>10.9</v>
       </c>
       <c r="P41" s="32">
         <f t="shared" si="4"/>
-        <v>3.2999999999999989</v>
+        <v>3.4000000000000004</v>
       </c>
       <c r="Q41" s="5">
         <f t="shared" si="5"/>
-        <v>36.499792407513674</v>
+        <v>37.526145216956387</v>
       </c>
     </row>
     <row r="42" spans="12:18">
-      <c r="M42" s="32"/>
-      <c r="N42" s="32"/>
-      <c r="O42" s="32"/>
+      <c r="L42">
+        <v>8</v>
+      </c>
+      <c r="M42" s="32">
+        <v>5</v>
+      </c>
+      <c r="N42" s="32">
+        <v>8.4</v>
+      </c>
+      <c r="O42" s="32">
+        <v>11.7</v>
+      </c>
       <c r="P42" s="32">
         <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="Q42" s="5" t="e">
+        <v>3.2999999999999989</v>
+      </c>
+      <c r="Q42" s="5">
         <f t="shared" si="5"/>
-        <v>#DIV/0!</v>
+        <v>36.499792407513674</v>
       </c>
     </row>
     <row r="43" spans="12:18">
@@ -2691,6 +2719,9 @@
       </c>
     </row>
     <row r="45" spans="12:18">
+      <c r="M45" s="32"/>
+      <c r="N45" s="32"/>
+      <c r="O45" s="32"/>
       <c r="P45" s="32">
         <f t="shared" si="4"/>
         <v>0</v>
@@ -2700,8 +2731,18 @@
         <v>#DIV/0!</v>
       </c>
     </row>
+    <row r="46" spans="12:18">
+      <c r="P46" s="32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Q46" s="5" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A5:K26"/>
+  <autoFilter ref="A5:K26" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <mergeCells count="4">
     <mergeCell ref="A1:A4"/>
     <mergeCell ref="D1:F1"/>
@@ -2709,37 +2750,37 @@
     <mergeCell ref="G1:G4"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A5" r:id="rId1" display="http://www.arducam.com/downloads/Lenses/LS40136.jpg"/>
-    <hyperlink ref="A6" r:id="rId2" display="http://www.arducam.com/downloads/Lenses/LS-40207.jpg"/>
-    <hyperlink ref="A7" r:id="rId3" display="http://www.arducam.com/downloads/Lenses/LS40166.JPG"/>
-    <hyperlink ref="A8" r:id="rId4" display="http://www.arducam.com/downloads/Lenses/LS-36021.jpg"/>
-    <hyperlink ref="A9" r:id="rId5" display="http://www.arducam.com/downloads/Lenses/HX1820.JPG"/>
-    <hyperlink ref="A10" r:id="rId6" display="http://www.arducam.com/downloads/Lenses/LS6020.JPG"/>
-    <hyperlink ref="A11" r:id="rId7" display="http://www.arducam.com/downloads/Lenses/LS8020.JPG"/>
-    <hyperlink ref="A12" r:id="rId8" display="http://www.arducam.com/downloads/Lenses/LS12020.JPG"/>
-    <hyperlink ref="A13" r:id="rId9" display="http://www.arducam.com/downloads/Lenses/LS1620.JPG"/>
-    <hyperlink ref="A14" r:id="rId10" display="http://www.arducam.com/downloads/Lenses/LS-30207.jpg"/>
-    <hyperlink ref="A15" r:id="rId11" display="http://www.arducam.com/downloads/Lenses/LS-27225.jpg"/>
-    <hyperlink ref="A16" r:id="rId12" display="http://www.arducam.com/downloads/Lenses/LS30188.JPG"/>
-    <hyperlink ref="A17" r:id="rId13" display="http://www.arducam.com/downloads/Lenses/LS-27227.jpg"/>
-    <hyperlink ref="A18" r:id="rId14" display="http://www.arducam.com/downloads/Lenses/LS-20211.jpg"/>
-    <hyperlink ref="A19" r:id="rId15" display="http://www.arducam.com/downloads/Lenses/LS20150.JPG"/>
-    <hyperlink ref="A20" r:id="rId16" display="http://www.arducam.com/downloads/Lenses/LS4014.JPG"/>
-    <hyperlink ref="A21" r:id="rId17" display="http://www.arducam.com/downloads/Lenses/LS-81600.jpg"/>
-    <hyperlink ref="A22" r:id="rId18" display="http://www.arducam.com/downloads/Lenses/Fisheye/HX-40146.pdf"/>
-    <hyperlink ref="A23" r:id="rId19" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS40180.JPG"/>
-    <hyperlink ref="A24" r:id="rId20" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS-30180.jpg"/>
-    <hyperlink ref="A25" r:id="rId21" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS25180.JPG"/>
-    <hyperlink ref="A26" r:id="rId22" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS-32220.pdf"/>
-    <hyperlink ref="R35" r:id="rId23"/>
-    <hyperlink ref="R27" r:id="rId24"/>
+    <hyperlink ref="A5" r:id="rId1" display="http://www.arducam.com/downloads/Lenses/LS40136.jpg" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A6" r:id="rId2" display="http://www.arducam.com/downloads/Lenses/LS-40207.jpg" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="A7" r:id="rId3" display="http://www.arducam.com/downloads/Lenses/LS40166.JPG" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="A8" r:id="rId4" display="http://www.arducam.com/downloads/Lenses/LS-36021.jpg" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="A9" r:id="rId5" display="http://www.arducam.com/downloads/Lenses/HX1820.JPG" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="A10" r:id="rId6" display="http://www.arducam.com/downloads/Lenses/LS6020.JPG" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="A11" r:id="rId7" display="http://www.arducam.com/downloads/Lenses/LS8020.JPG" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="A12" r:id="rId8" display="http://www.arducam.com/downloads/Lenses/LS12020.JPG" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="A13" r:id="rId9" display="http://www.arducam.com/downloads/Lenses/LS1620.JPG" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="A14" r:id="rId10" display="http://www.arducam.com/downloads/Lenses/LS-30207.jpg" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="A15" r:id="rId11" display="http://www.arducam.com/downloads/Lenses/LS-27225.jpg" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="A16" r:id="rId12" display="http://www.arducam.com/downloads/Lenses/LS30188.JPG" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="A17" r:id="rId13" display="http://www.arducam.com/downloads/Lenses/LS-27227.jpg" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="A18" r:id="rId14" display="http://www.arducam.com/downloads/Lenses/LS-20211.jpg" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="A19" r:id="rId15" display="http://www.arducam.com/downloads/Lenses/LS20150.JPG" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="A20" r:id="rId16" display="http://www.arducam.com/downloads/Lenses/LS4014.JPG" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="A21" r:id="rId17" display="http://www.arducam.com/downloads/Lenses/LS-81600.jpg" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="A22" r:id="rId18" display="http://www.arducam.com/downloads/Lenses/Fisheye/HX-40146.pdf" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="A23" r:id="rId19" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS40180.JPG" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="A24" r:id="rId20" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS-30180.jpg" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="A25" r:id="rId21" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS25180.JPG" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="A26" r:id="rId22" display="http://www.arducam.com/downloads/Lenses/Fisheye/LS-32220.pdf" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="R36" r:id="rId23" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="R27" r:id="rId24" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A2:F26"/>
   <sheetViews>
@@ -2917,8 +2958,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A26" r:id="rId1"/>
-    <hyperlink ref="A25" r:id="rId2"/>
+    <hyperlink ref="A26" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="A25" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId3"/>

</xml_diff>